<commit_message>
Crar segunda prueba de escritorio
</commit_message>
<xml_diff>
--- a/Tabla pruebas de escritorio.xlsx
+++ b/Tabla pruebas de escritorio.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gurdian0614\Documents\Pseint\Pruebas-Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1650DB2-1721-4A8D-B564-2E0F4015DE72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7595D27-820A-4189-B45E-FA76865A8C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3771B2A4-4203-45F6-B05B-3C2E5BAAFD62}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{3771B2A4-4203-45F6-B05B-3C2E5BAAFD62}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ejercicio 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ejercicio 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="48">
   <si>
     <t>n1</t>
   </si>
@@ -111,6 +112,75 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>division</t>
+  </si>
+  <si>
+    <t>modulo</t>
+  </si>
+  <si>
+    <t>num1</t>
+  </si>
+  <si>
+    <t>num2</t>
+  </si>
+  <si>
+    <t>1:EJERCICIO_26(1)</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Variable no inicializada (DIVISION).&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Variable no inicializada (MODULO).&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Variable no inicializada (NUM1).&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Variable no inicializada (NUM2).&gt;&gt;</t>
+  </si>
+  <si>
+    <t>1:EJERCICIO_27(1)</t>
+  </si>
+  <si>
+    <t>1:EJERCICIO_29(1)</t>
+  </si>
+  <si>
+    <t>1:EJERCICIO_210(1)</t>
+  </si>
+  <si>
+    <t>1:EJERCICIO_211(1)</t>
+  </si>
+  <si>
+    <t>1:EJERCICIO_212(1)</t>
+  </si>
+  <si>
+    <t>1:EJERCICIO_214(1)</t>
+  </si>
+  <si>
+    <t>1:EJERCICIO_215(1)</t>
+  </si>
+  <si>
+    <t>1:EJERCICIO_222(1)</t>
+  </si>
+  <si>
+    <t>1:EJERCICIO_223(1)</t>
+  </si>
+  <si>
+    <t>1:EJERCICIO_216(1)</t>
+  </si>
+  <si>
+    <t>1:EJERCICIO_217(1)</t>
+  </si>
+  <si>
+    <t>1:EJERCICIO_218(1)</t>
+  </si>
+  <si>
+    <t>1:EJERCICIO_220(1)</t>
+  </si>
+  <si>
+    <t>1:EJERCICIO_221(1)</t>
   </si>
 </sst>
 </file>
@@ -516,7 +586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0B825AF-7BF6-4A1D-8B03-6F3C42C81143}">
   <dimension ref="B3:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -815,4 +885,482 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2DA0E70-1C4B-4608-995B-E4474759CE3C}">
+  <dimension ref="C2:H30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="34.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="1">
+        <v>10</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="1">
+        <v>10</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" s="1">
+        <v>10</v>
+      </c>
+      <c r="G23" s="1">
+        <v>2</v>
+      </c>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="1">
+        <v>10</v>
+      </c>
+      <c r="G24" s="1">
+        <v>2</v>
+      </c>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C25" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="1">
+        <v>10</v>
+      </c>
+      <c r="G25" s="1">
+        <v>2</v>
+      </c>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="1">
+        <v>5</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="1">
+        <v>10</v>
+      </c>
+      <c r="G26" s="1">
+        <v>2</v>
+      </c>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C27" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="1">
+        <v>5</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>10</v>
+      </c>
+      <c r="G27" s="1">
+        <v>2</v>
+      </c>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C28" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="1">
+        <v>5</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1">
+        <v>10</v>
+      </c>
+      <c r="G28" s="1">
+        <v>2</v>
+      </c>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C29" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="1">
+        <v>5</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1">
+        <v>10</v>
+      </c>
+      <c r="G29" s="1">
+        <v>2</v>
+      </c>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C30" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="1">
+        <v>5</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1">
+        <v>10</v>
+      </c>
+      <c r="G30" s="1">
+        <v>2</v>
+      </c>
+      <c r="H30" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>